<commit_message>
Disabled user interaction while running
</commit_message>
<xml_diff>
--- a/templateNew.xlsx
+++ b/templateNew.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Kai\Desktop\TimeSheet\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{D2ED3DFF-9C46-4897-A0F6-8F55C5F91FC1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{4FE2D233-F2ED-4B7F-BEBA-9793AC01D5AD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1520" yWindow="1520" windowWidth="19200" windowHeight="10060" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="380" yWindow="380" windowWidth="19200" windowHeight="10060" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="999" sheetId="3" r:id="rId1"/>
@@ -129,7 +129,7 @@
     <t>VERY GOOD BUILDING COMPANY</t>
   </si>
   <si>
-    <t>MAY</t>
+    <t>APRIL</t>
   </si>
 </sst>
 </file>
@@ -758,7 +758,7 @@
       <c r="G7" s="17"/>
       <c r="H7" s="17" t="str">
         <f>COUNTA(Formulas!H2:H30) &amp; " DAYS"</f>
-        <v>23 DAYS</v>
+        <v>22 DAYS</v>
       </c>
     </row>
     <row r="8" spans="1:8" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
@@ -842,10 +842,10 @@
     <row r="12" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A12" s="21" cm="1">
         <f t="array" ref="A12:B35">_xlfn._xlws.FILTER(IF(Formulas!$J$2:'Formulas'!$K$31&lt;&gt;0, Formulas!$J$2:'Formulas'!$K$31, ""), (ROW(Formulas!$J$2:'Formulas'!$J$31) &lt;= MAX(_xlfn._xlws.FILTER(ROW(Formulas!$J$2:'Formulas'!$J$31), Formulas!$J$2:'Formulas'!$J$31&lt;&gt;""))))</f>
-        <v>45413</v>
+        <v>45383</v>
       </c>
       <c r="B12" s="16">
-        <v>45413</v>
+        <v>45383</v>
       </c>
       <c r="C12" s="1"/>
       <c r="D12" s="1"/>
@@ -856,138 +856,138 @@
     </row>
     <row r="13" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A13" s="21">
-        <v>45414</v>
+        <v>45384</v>
       </c>
       <c r="B13" s="16">
-        <v>45414</v>
+        <v>45384</v>
       </c>
     </row>
     <row r="14" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A14" s="21">
-        <v>45415</v>
+        <v>45385</v>
       </c>
       <c r="B14" s="16">
-        <v>45415</v>
+        <v>45385</v>
       </c>
     </row>
     <row r="15" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A15" s="21">
-        <v>45418</v>
+        <v>45386</v>
       </c>
       <c r="B15" s="16">
-        <v>45418</v>
+        <v>45386</v>
       </c>
     </row>
     <row r="16" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A16" s="21">
-        <v>45419</v>
+        <v>45387</v>
       </c>
       <c r="B16" s="16">
-        <v>45419</v>
+        <v>45387</v>
       </c>
     </row>
     <row r="17" spans="1:2" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A17" s="21">
-        <v>45420</v>
+        <v>45390</v>
       </c>
       <c r="B17" s="16">
-        <v>45420</v>
+        <v>45390</v>
       </c>
     </row>
     <row r="18" spans="1:2" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A18" s="21">
-        <v>45421</v>
+        <v>45391</v>
       </c>
       <c r="B18" s="16">
-        <v>45421</v>
+        <v>45391</v>
       </c>
     </row>
     <row r="19" spans="1:2" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A19" s="21">
-        <v>45422</v>
+        <v>45392</v>
       </c>
       <c r="B19" s="16">
-        <v>45422</v>
+        <v>45392</v>
       </c>
     </row>
     <row r="20" spans="1:2" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A20" s="21">
-        <v>45425</v>
+        <v>45393</v>
       </c>
       <c r="B20" s="16">
-        <v>45425</v>
+        <v>45393</v>
       </c>
     </row>
     <row r="21" spans="1:2" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A21" s="21">
-        <v>45426</v>
+        <v>45394</v>
       </c>
       <c r="B21" s="16">
-        <v>45426</v>
+        <v>45394</v>
       </c>
     </row>
     <row r="22" spans="1:2" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A22" s="21">
-        <v>45427</v>
+        <v>45397</v>
       </c>
       <c r="B22" s="16">
-        <v>45427</v>
+        <v>45397</v>
       </c>
     </row>
     <row r="23" spans="1:2" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A23" s="21">
-        <v>45428</v>
+        <v>45398</v>
       </c>
       <c r="B23" s="16">
-        <v>45428</v>
+        <v>45398</v>
       </c>
     </row>
     <row r="24" spans="1:2" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A24" s="21">
-        <v>45429</v>
+        <v>45399</v>
       </c>
       <c r="B24" s="16">
-        <v>45429</v>
+        <v>45399</v>
       </c>
     </row>
     <row r="25" spans="1:2" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A25" s="21">
-        <v>45432</v>
+        <v>45400</v>
       </c>
       <c r="B25" s="16">
-        <v>45432</v>
+        <v>45400</v>
       </c>
     </row>
     <row r="26" spans="1:2" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A26" s="21">
-        <v>45433</v>
+        <v>45401</v>
       </c>
       <c r="B26" s="16">
-        <v>45433</v>
+        <v>45401</v>
       </c>
     </row>
     <row r="27" spans="1:2" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A27" s="21">
-        <v>45434</v>
+        <v>45404</v>
       </c>
       <c r="B27" s="16">
-        <v>45434</v>
+        <v>45404</v>
       </c>
     </row>
     <row r="28" spans="1:2" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A28" s="21">
-        <v>45435</v>
+        <v>45405</v>
       </c>
       <c r="B28" s="16">
-        <v>45435</v>
+        <v>45405</v>
       </c>
     </row>
     <row r="29" spans="1:2" ht="30" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A29" s="21">
-        <v>45436</v>
-      </c>
-      <c r="B29" s="16">
-        <v>45436</v>
+      <c r="A29" s="21" t="str">
+        <v/>
+      </c>
+      <c r="B29" s="16" t="str">
+        <v/>
       </c>
     </row>
     <row r="30" spans="1:2" ht="30" customHeight="1" x14ac:dyDescent="0.35">
@@ -1000,42 +1000,42 @@
     </row>
     <row r="31" spans="1:2" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A31" s="23">
-        <v>45439</v>
+        <v>45406</v>
       </c>
       <c r="B31" s="16">
-        <v>45439</v>
+        <v>45406</v>
       </c>
     </row>
     <row r="32" spans="1:2" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A32" s="23">
-        <v>45440</v>
+        <v>45407</v>
       </c>
       <c r="B32" s="16">
-        <v>45440</v>
+        <v>45407</v>
       </c>
     </row>
     <row r="33" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A33" s="23">
-        <v>45441</v>
+        <v>45408</v>
       </c>
       <c r="B33" s="16">
-        <v>45441</v>
+        <v>45408</v>
       </c>
     </row>
     <row r="34" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A34" s="21">
-        <v>45442</v>
+        <v>45411</v>
       </c>
       <c r="B34" s="22">
-        <v>45442</v>
+        <v>45411</v>
       </c>
     </row>
     <row r="35" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A35" s="23">
-        <v>45443</v>
+        <v>45412</v>
       </c>
       <c r="B35" s="16">
-        <v>45443</v>
+        <v>45412</v>
       </c>
     </row>
     <row r="36" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.35">
@@ -3926,7 +3926,7 @@
     <row r="1" spans="2:11" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B1" s="36">
         <f>DATEVALUE('999'!$F$8 &amp; " 1, " &amp; '999'!$H$8)</f>
-        <v>45413</v>
+        <v>45383</v>
       </c>
       <c r="C1" s="36"/>
       <c r="E1" s="37" t="s">
@@ -3951,26 +3951,26 @@
         <v>1</v>
       </c>
       <c r="E2" s="25" cm="1">
-        <f t="array" ref="E2:E32">IF(B8=FALSE, _xlfn.SEQUENCE(DAY(EOMONTH(B1,0)), 1,B1, 1), "")</f>
-        <v>45413</v>
+        <f t="array" ref="E2:E31">IF(B8=FALSE, _xlfn.SEQUENCE(DAY(EOMONTH(B1,0)), 1,B1, 1), "")</f>
+        <v>45383</v>
       </c>
       <c r="F2" s="27">
         <f>IF($E2="","",WEEKDAY($E2)-1)</f>
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="G2" s="6"/>
       <c r="H2" s="25" cm="1">
-        <f t="array" ref="H2:H24">_xlfn._xlws.FILTER($E$2:$E$32, ($F$2:$F$32=$C$2)+($F$2:$F$32=$C$3)+($F$2:$F$32=$C$4)+($F$2:$F$32=$C$5)+($F$2:$F$32=$C$6)+($F$2:$F$32=$C$7), "")</f>
-        <v>45413</v>
+        <f t="array" ref="H2:H23">_xlfn._xlws.FILTER($E$2:$E$32, ($F$2:$F$32=$C$2)+($F$2:$F$32=$C$3)+($F$2:$F$32=$C$4)+($F$2:$F$32=$C$5)+($F$2:$F$32=$C$6)+($F$2:$F$32=$C$7), "")</f>
+        <v>45383</v>
       </c>
       <c r="I2" s="6"/>
       <c r="J2" s="19" cm="1">
-        <f t="array" ref="J2:J19">IF(OR(ISBLANK($H$21), $H$26&lt;&gt;""), _xlfn._xlws.FILTER($H$2:$H$32, (ROW($H$2:$H$32)&lt;21)*($H$2:$H$32&lt;&gt;"")), _xlfn._xlws.FILTER($H$2:$H$32, (ROW($H$2:$H$32)&lt;=COUNT($H$2:$H$32)-4)*($H$2:$H$32&lt;&gt;"")))</f>
-        <v>45413</v>
+        <f t="array" ref="J2:J18">IF(OR(ISBLANK($H$21), $H$26&lt;&gt;""), _xlfn._xlws.FILTER($H$2:$H$32, (ROW($H$2:$H$32)&lt;21)*($H$2:$H$32&lt;&gt;"")), _xlfn._xlws.FILTER($H$2:$H$32, (ROW($H$2:$H$32)&lt;=COUNT($H$2:$H$32)-4)*($H$2:$H$32&lt;&gt;"")))</f>
+        <v>45383</v>
       </c>
       <c r="K2" s="13" cm="1">
-        <f t="array" ref="K2:K19">IF(OR(ISBLANK($H$21), $H$26&lt;&gt;""), _xlfn._xlws.FILTER($H$2:$H$32, (ROW($H$2:$H$32)&lt;21)*($H$2:$H$32&lt;&gt;"")), _xlfn._xlws.FILTER($H$2:$H$32, (ROW($H$2:$H$32)&lt;=COUNT($H$2:$H$32)-4)*($H$2:$H$32&lt;&gt;"")))</f>
-        <v>45413</v>
+        <f t="array" ref="K2:K18">IF(OR(ISBLANK($H$21), $H$26&lt;&gt;""), _xlfn._xlws.FILTER($H$2:$H$32, (ROW($H$2:$H$32)&lt;21)*($H$2:$H$32&lt;&gt;"")), _xlfn._xlws.FILTER($H$2:$H$32, (ROW($H$2:$H$32)&lt;=COUNT($H$2:$H$32)-4)*($H$2:$H$32&lt;&gt;"")))</f>
+        <v>45383</v>
       </c>
     </row>
     <row r="3" spans="2:11" ht="14.5" x14ac:dyDescent="0.35">
@@ -3982,22 +3982,22 @@
         <v>2</v>
       </c>
       <c r="E3" s="4">
-        <v>45414</v>
+        <v>45384</v>
       </c>
       <c r="F3" s="5">
         <f t="shared" ref="F3:F32" si="1">IF($E3="","",WEEKDAY($E3)-1)</f>
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="G3" s="6"/>
       <c r="H3" s="4">
-        <v>45414</v>
+        <v>45384</v>
       </c>
       <c r="I3" s="6"/>
       <c r="J3" s="19">
-        <v>45414</v>
+        <v>45384</v>
       </c>
       <c r="K3" s="13">
-        <v>45414</v>
+        <v>45384</v>
       </c>
     </row>
     <row r="4" spans="2:11" ht="14.5" x14ac:dyDescent="0.35">
@@ -4009,22 +4009,22 @@
         <v>3</v>
       </c>
       <c r="E4" s="4">
-        <v>45415</v>
+        <v>45385</v>
       </c>
       <c r="F4" s="5">
         <f t="shared" si="1"/>
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="G4" s="6"/>
       <c r="H4" s="4">
-        <v>45415</v>
+        <v>45385</v>
       </c>
       <c r="I4" s="6"/>
       <c r="J4" s="19">
-        <v>45415</v>
+        <v>45385</v>
       </c>
       <c r="K4" s="13">
-        <v>45415</v>
+        <v>45385</v>
       </c>
     </row>
     <row r="5" spans="2:11" ht="14.5" x14ac:dyDescent="0.35">
@@ -4036,22 +4036,22 @@
         <v>4</v>
       </c>
       <c r="E5" s="4">
-        <v>45416</v>
+        <v>45386</v>
       </c>
       <c r="F5" s="5">
         <f t="shared" si="1"/>
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="G5" s="6"/>
       <c r="H5" s="4">
-        <v>45418</v>
+        <v>45386</v>
       </c>
       <c r="I5" s="6"/>
       <c r="J5" s="19">
-        <v>45418</v>
+        <v>45386</v>
       </c>
       <c r="K5" s="13">
-        <v>45418</v>
+        <v>45386</v>
       </c>
     </row>
     <row r="6" spans="2:11" ht="14.5" x14ac:dyDescent="0.35">
@@ -4063,22 +4063,22 @@
         <v>5</v>
       </c>
       <c r="E6" s="4">
-        <v>45417</v>
+        <v>45387</v>
       </c>
       <c r="F6" s="5">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="G6" s="6"/>
       <c r="H6" s="4">
-        <v>45419</v>
+        <v>45387</v>
       </c>
       <c r="I6" s="6"/>
       <c r="J6" s="19">
-        <v>45419</v>
+        <v>45387</v>
       </c>
       <c r="K6" s="13">
-        <v>45419</v>
+        <v>45387</v>
       </c>
     </row>
     <row r="7" spans="2:11" ht="14.5" x14ac:dyDescent="0.35">
@@ -4088,22 +4088,22 @@
         <v>-1</v>
       </c>
       <c r="E7" s="4">
-        <v>45418</v>
+        <v>45388</v>
       </c>
       <c r="F7" s="5">
         <f t="shared" si="1"/>
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="G7" s="6"/>
       <c r="H7" s="4">
-        <v>45420</v>
+        <v>45390</v>
       </c>
       <c r="I7" s="6"/>
       <c r="J7" s="19">
-        <v>45420</v>
+        <v>45390</v>
       </c>
       <c r="K7" s="13">
-        <v>45420</v>
+        <v>45390</v>
       </c>
     </row>
     <row r="8" spans="2:11" ht="14.5" x14ac:dyDescent="0.35">
@@ -4113,257 +4113,253 @@
       </c>
       <c r="C8" s="39"/>
       <c r="E8" s="4">
-        <v>45419</v>
+        <v>45389</v>
       </c>
       <c r="F8" s="5">
         <f t="shared" si="1"/>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="G8" s="6"/>
       <c r="H8" s="4">
-        <v>45421</v>
+        <v>45391</v>
       </c>
       <c r="I8" s="6"/>
       <c r="J8" s="19">
-        <v>45421</v>
+        <v>45391</v>
       </c>
       <c r="K8" s="13">
-        <v>45421</v>
+        <v>45391</v>
       </c>
     </row>
     <row r="9" spans="2:11" ht="14.5" x14ac:dyDescent="0.35">
       <c r="B9" s="39"/>
       <c r="C9" s="39"/>
       <c r="E9" s="4">
-        <v>45420</v>
+        <v>45390</v>
       </c>
       <c r="F9" s="5">
         <f t="shared" si="1"/>
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="G9" s="6"/>
       <c r="H9" s="4">
-        <v>45422</v>
+        <v>45392</v>
       </c>
       <c r="I9" s="6"/>
       <c r="J9" s="19">
-        <v>45422</v>
+        <v>45392</v>
       </c>
       <c r="K9" s="13">
-        <v>45422</v>
+        <v>45392</v>
       </c>
     </row>
     <row r="10" spans="2:11" ht="14.5" x14ac:dyDescent="0.35">
       <c r="E10" s="4">
-        <v>45421</v>
+        <v>45391</v>
       </c>
       <c r="F10" s="5">
         <f t="shared" si="1"/>
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="G10" s="6"/>
       <c r="H10" s="4">
-        <v>45425</v>
+        <v>45393</v>
       </c>
       <c r="I10" s="6"/>
       <c r="J10" s="19">
-        <v>45425</v>
+        <v>45393</v>
       </c>
       <c r="K10" s="13">
-        <v>45425</v>
+        <v>45393</v>
       </c>
     </row>
     <row r="11" spans="2:11" ht="14.5" x14ac:dyDescent="0.35">
       <c r="E11" s="4">
-        <v>45422</v>
+        <v>45392</v>
       </c>
       <c r="F11" s="5">
         <f t="shared" si="1"/>
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="G11" s="6"/>
       <c r="H11" s="4">
-        <v>45426</v>
+        <v>45394</v>
       </c>
       <c r="I11" s="6"/>
       <c r="J11" s="19">
-        <v>45426</v>
+        <v>45394</v>
       </c>
       <c r="K11" s="13">
-        <v>45426</v>
+        <v>45394</v>
       </c>
     </row>
     <row r="12" spans="2:11" ht="14.5" x14ac:dyDescent="0.35">
       <c r="E12" s="4">
-        <v>45423</v>
+        <v>45393</v>
       </c>
       <c r="F12" s="5">
         <f t="shared" si="1"/>
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="G12" s="6"/>
       <c r="H12" s="4">
-        <v>45427</v>
+        <v>45397</v>
       </c>
       <c r="I12" s="6"/>
       <c r="J12" s="19">
-        <v>45427</v>
+        <v>45397</v>
       </c>
       <c r="K12" s="13">
-        <v>45427</v>
+        <v>45397</v>
       </c>
     </row>
     <row r="13" spans="2:11" ht="14.5" x14ac:dyDescent="0.35">
       <c r="E13" s="4">
-        <v>45424</v>
+        <v>45394</v>
       </c>
       <c r="F13" s="5">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="G13" s="6"/>
       <c r="H13" s="4">
-        <v>45428</v>
+        <v>45398</v>
       </c>
       <c r="I13" s="6"/>
       <c r="J13" s="19">
-        <v>45428</v>
+        <v>45398</v>
       </c>
       <c r="K13" s="13">
-        <v>45428</v>
+        <v>45398</v>
       </c>
     </row>
     <row r="14" spans="2:11" ht="14.5" x14ac:dyDescent="0.35">
       <c r="E14" s="4">
-        <v>45425</v>
+        <v>45395</v>
       </c>
       <c r="F14" s="5">
         <f t="shared" si="1"/>
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="G14" s="6"/>
       <c r="H14" s="4">
-        <v>45429</v>
+        <v>45399</v>
       </c>
       <c r="I14" s="6"/>
       <c r="J14" s="19">
-        <v>45429</v>
+        <v>45399</v>
       </c>
       <c r="K14" s="13">
-        <v>45429</v>
+        <v>45399</v>
       </c>
     </row>
     <row r="15" spans="2:11" ht="14.5" x14ac:dyDescent="0.35">
       <c r="E15" s="4">
-        <v>45426</v>
+        <v>45396</v>
       </c>
       <c r="F15" s="5">
         <f t="shared" si="1"/>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="G15" s="6"/>
       <c r="H15" s="4">
-        <v>45432</v>
+        <v>45400</v>
       </c>
       <c r="I15" s="6"/>
       <c r="J15" s="19">
-        <v>45432</v>
+        <v>45400</v>
       </c>
       <c r="K15" s="13">
-        <v>45432</v>
+        <v>45400</v>
       </c>
     </row>
     <row r="16" spans="2:11" ht="14.5" x14ac:dyDescent="0.35">
       <c r="E16" s="4">
-        <v>45427</v>
+        <v>45397</v>
       </c>
       <c r="F16" s="5">
         <f t="shared" si="1"/>
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="G16" s="6"/>
       <c r="H16" s="4">
-        <v>45433</v>
+        <v>45401</v>
       </c>
       <c r="I16" s="6"/>
       <c r="J16" s="19">
-        <v>45433</v>
+        <v>45401</v>
       </c>
       <c r="K16" s="13">
-        <v>45433</v>
+        <v>45401</v>
       </c>
     </row>
     <row r="17" spans="5:11" ht="14.5" x14ac:dyDescent="0.35">
       <c r="E17" s="4">
-        <v>45428</v>
+        <v>45398</v>
       </c>
       <c r="F17" s="5">
         <f t="shared" si="1"/>
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="G17" s="6"/>
       <c r="H17" s="4">
-        <v>45434</v>
+        <v>45404</v>
       </c>
       <c r="I17" s="6"/>
       <c r="J17" s="19">
-        <v>45434</v>
+        <v>45404</v>
       </c>
       <c r="K17" s="13">
-        <v>45434</v>
+        <v>45404</v>
       </c>
     </row>
     <row r="18" spans="5:11" ht="14.5" x14ac:dyDescent="0.35">
       <c r="E18" s="4">
-        <v>45429</v>
+        <v>45399</v>
       </c>
       <c r="F18" s="5">
         <f t="shared" si="1"/>
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="G18" s="6"/>
       <c r="H18" s="4">
-        <v>45435</v>
+        <v>45405</v>
       </c>
       <c r="I18" s="6"/>
       <c r="J18" s="19">
-        <v>45435</v>
+        <v>45405</v>
       </c>
       <c r="K18" s="13">
-        <v>45435</v>
+        <v>45405</v>
       </c>
     </row>
     <row r="19" spans="5:11" ht="14.5" x14ac:dyDescent="0.35">
       <c r="E19" s="4">
-        <v>45430</v>
+        <v>45400</v>
       </c>
       <c r="F19" s="5">
         <f t="shared" si="1"/>
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="G19" s="6"/>
       <c r="H19" s="4">
-        <v>45436</v>
+        <v>45406</v>
       </c>
       <c r="I19" s="6"/>
-      <c r="J19" s="19">
-        <v>45436</v>
-      </c>
-      <c r="K19" s="13">
-        <v>45436</v>
-      </c>
+      <c r="J19" s="19"/>
+      <c r="K19" s="13"/>
     </row>
     <row r="20" spans="5:11" ht="14.5" x14ac:dyDescent="0.35">
       <c r="E20" s="4">
-        <v>45431</v>
+        <v>45401</v>
       </c>
       <c r="F20" s="5">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="G20" s="6"/>
       <c r="H20" s="4">
-        <v>45439</v>
+        <v>45407</v>
       </c>
       <c r="I20" s="6"/>
       <c r="J20" s="19"/>
@@ -4371,111 +4367,109 @@
     </row>
     <row r="21" spans="5:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E21" s="4">
-        <v>45432</v>
+        <v>45402</v>
       </c>
       <c r="F21" s="5">
         <f t="shared" si="1"/>
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="G21" s="6"/>
       <c r="H21" s="4">
-        <v>45440</v>
+        <v>45408</v>
       </c>
       <c r="I21" s="6"/>
       <c r="J21" s="19" cm="1">
         <f t="array" ref="J21:J25">IF(ISBLANK($H$21),"",IF(ISBLANK($H$26), _xlfn._xlws.FILTER($H$2:$H$32, (ROW($H$2:$H$32)&gt;COUNT($H$2:$H$32)-4)*($H$2:$H$32&lt;&gt;"")),_xlfn._xlws.FILTER($H$2:$H$32, (ROW($H$2:$H$32)&gt;=21)*($H$2:$H$32&lt;&gt;""))))</f>
-        <v>45439</v>
+        <v>45406</v>
       </c>
       <c r="K21" s="13" cm="1">
         <f t="array" ref="K21:K25">IF(ISBLANK($H$21),"",IF(ISBLANK($H$26), _xlfn._xlws.FILTER($H$2:$H$32, (ROW($H$2:$H$32)&gt;COUNT($H$2:$H$32)-4)*($H$2:$H$32&lt;&gt;"")),_xlfn._xlws.FILTER($H$2:$H$32, (ROW($H$2:$H$32)&gt;=20)*($H$2:$H$32&lt;&gt;""))))</f>
-        <v>45439</v>
+        <v>45406</v>
       </c>
     </row>
     <row r="22" spans="5:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E22" s="4">
-        <v>45433</v>
+        <v>45403</v>
       </c>
       <c r="F22" s="5">
         <f t="shared" si="1"/>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="G22" s="6"/>
       <c r="H22" s="4">
-        <v>45441</v>
+        <v>45411</v>
       </c>
       <c r="I22" s="6"/>
       <c r="J22" s="19">
-        <v>45440</v>
+        <v>45407</v>
       </c>
       <c r="K22" s="13">
-        <v>45440</v>
+        <v>45407</v>
       </c>
     </row>
     <row r="23" spans="5:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E23" s="4">
-        <v>45434</v>
+        <v>45404</v>
       </c>
       <c r="F23" s="5">
         <f t="shared" si="1"/>
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="G23" s="6"/>
       <c r="H23" s="4">
-        <v>45442</v>
+        <v>45412</v>
       </c>
       <c r="I23" s="6"/>
       <c r="J23" s="19">
-        <v>45441</v>
+        <v>45408</v>
       </c>
       <c r="K23" s="13">
-        <v>45441</v>
+        <v>45408</v>
       </c>
     </row>
     <row r="24" spans="5:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E24" s="4">
-        <v>45435</v>
+        <v>45405</v>
       </c>
       <c r="F24" s="5">
         <f t="shared" si="1"/>
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="G24" s="6"/>
-      <c r="H24" s="4">
-        <v>45443</v>
-      </c>
+      <c r="H24" s="4"/>
       <c r="I24" s="6"/>
       <c r="J24" s="19">
-        <v>45442</v>
+        <v>45411</v>
       </c>
       <c r="K24" s="13">
-        <v>45442</v>
+        <v>45411</v>
       </c>
     </row>
     <row r="25" spans="5:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E25" s="4">
-        <v>45436</v>
+        <v>45406</v>
       </c>
       <c r="F25" s="5">
         <f t="shared" si="1"/>
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="G25" s="6"/>
       <c r="H25" s="4"/>
       <c r="I25" s="6"/>
       <c r="J25" s="19">
-        <v>45443</v>
+        <v>45412</v>
       </c>
       <c r="K25" s="13">
-        <v>45443</v>
+        <v>45412</v>
       </c>
     </row>
     <row r="26" spans="5:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E26" s="4">
-        <v>45437</v>
+        <v>45407</v>
       </c>
       <c r="F26" s="5">
         <f t="shared" si="1"/>
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="G26" s="6"/>
       <c r="H26" s="4"/>
@@ -4485,11 +4479,11 @@
     </row>
     <row r="27" spans="5:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E27" s="4">
-        <v>45438</v>
+        <v>45408</v>
       </c>
       <c r="F27" s="5">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="G27" s="6"/>
       <c r="H27" s="4"/>
@@ -4499,11 +4493,11 @@
     </row>
     <row r="28" spans="5:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E28" s="4">
-        <v>45439</v>
+        <v>45409</v>
       </c>
       <c r="F28" s="5">
         <f t="shared" si="1"/>
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="G28" s="6"/>
       <c r="H28" s="4"/>
@@ -4513,11 +4507,11 @@
     </row>
     <row r="29" spans="5:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E29" s="4">
-        <v>45440</v>
+        <v>45410</v>
       </c>
       <c r="F29" s="5">
         <f t="shared" si="1"/>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="G29" s="6"/>
       <c r="H29" s="4"/>
@@ -4527,11 +4521,11 @@
     </row>
     <row r="30" spans="5:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E30" s="4">
-        <v>45441</v>
+        <v>45411</v>
       </c>
       <c r="F30" s="5">
         <f t="shared" si="1"/>
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="G30" s="6"/>
       <c r="H30" s="4"/>
@@ -4541,11 +4535,11 @@
     </row>
     <row r="31" spans="5:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E31" s="4">
-        <v>45442</v>
+        <v>45412</v>
       </c>
       <c r="F31" s="5">
         <f t="shared" si="1"/>
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="G31" s="6"/>
       <c r="H31" s="4"/>
@@ -4554,12 +4548,10 @@
       <c r="K31" s="13"/>
     </row>
     <row r="32" spans="5:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="E32" s="4">
-        <v>45443</v>
-      </c>
-      <c r="F32" s="5">
+      <c r="E32" s="4"/>
+      <c r="F32" s="5" t="str">
         <f t="shared" si="1"/>
-        <v>5</v>
+        <v/>
       </c>
       <c r="G32" s="6"/>
       <c r="H32" s="4"/>

</xml_diff>

<commit_message>
Buttons functionality changed to toggles to stop processes
</commit_message>
<xml_diff>
--- a/templateNew.xlsx
+++ b/templateNew.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Kai\Desktop\TimeSheet\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{4FE2D233-F2ED-4B7F-BEBA-9793AC01D5AD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{4D73AB3B-8D0F-484D-BF62-8271640986ED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="380" yWindow="380" windowWidth="19200" windowHeight="10060" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3040" yWindow="3040" windowWidth="19200" windowHeight="10060" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="999" sheetId="3" r:id="rId1"/>
@@ -129,7 +129,7 @@
     <t>VERY GOOD BUILDING COMPANY</t>
   </si>
   <si>
-    <t>APRIL</t>
+    <t>MAY</t>
   </si>
 </sst>
 </file>
@@ -758,7 +758,7 @@
       <c r="G7" s="17"/>
       <c r="H7" s="17" t="str">
         <f>COUNTA(Formulas!H2:H30) &amp; " DAYS"</f>
-        <v>22 DAYS</v>
+        <v>23 DAYS</v>
       </c>
     </row>
     <row r="8" spans="1:8" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
@@ -842,10 +842,10 @@
     <row r="12" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A12" s="21" cm="1">
         <f t="array" ref="A12:B35">_xlfn._xlws.FILTER(IF(Formulas!$J$2:'Formulas'!$K$31&lt;&gt;0, Formulas!$J$2:'Formulas'!$K$31, ""), (ROW(Formulas!$J$2:'Formulas'!$J$31) &lt;= MAX(_xlfn._xlws.FILTER(ROW(Formulas!$J$2:'Formulas'!$J$31), Formulas!$J$2:'Formulas'!$J$31&lt;&gt;""))))</f>
-        <v>45383</v>
+        <v>45413</v>
       </c>
       <c r="B12" s="16">
-        <v>45383</v>
+        <v>45413</v>
       </c>
       <c r="C12" s="1"/>
       <c r="D12" s="1"/>
@@ -856,138 +856,138 @@
     </row>
     <row r="13" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A13" s="21">
-        <v>45384</v>
+        <v>45414</v>
       </c>
       <c r="B13" s="16">
-        <v>45384</v>
+        <v>45414</v>
       </c>
     </row>
     <row r="14" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A14" s="21">
-        <v>45385</v>
+        <v>45415</v>
       </c>
       <c r="B14" s="16">
-        <v>45385</v>
+        <v>45415</v>
       </c>
     </row>
     <row r="15" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A15" s="21">
-        <v>45386</v>
+        <v>45418</v>
       </c>
       <c r="B15" s="16">
-        <v>45386</v>
+        <v>45418</v>
       </c>
     </row>
     <row r="16" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A16" s="21">
-        <v>45387</v>
+        <v>45419</v>
       </c>
       <c r="B16" s="16">
-        <v>45387</v>
+        <v>45419</v>
       </c>
     </row>
     <row r="17" spans="1:2" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A17" s="21">
-        <v>45390</v>
+        <v>45420</v>
       </c>
       <c r="B17" s="16">
-        <v>45390</v>
+        <v>45420</v>
       </c>
     </row>
     <row r="18" spans="1:2" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A18" s="21">
-        <v>45391</v>
+        <v>45421</v>
       </c>
       <c r="B18" s="16">
-        <v>45391</v>
+        <v>45421</v>
       </c>
     </row>
     <row r="19" spans="1:2" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A19" s="21">
-        <v>45392</v>
+        <v>45422</v>
       </c>
       <c r="B19" s="16">
-        <v>45392</v>
+        <v>45422</v>
       </c>
     </row>
     <row r="20" spans="1:2" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A20" s="21">
-        <v>45393</v>
+        <v>45425</v>
       </c>
       <c r="B20" s="16">
-        <v>45393</v>
+        <v>45425</v>
       </c>
     </row>
     <row r="21" spans="1:2" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A21" s="21">
-        <v>45394</v>
+        <v>45426</v>
       </c>
       <c r="B21" s="16">
-        <v>45394</v>
+        <v>45426</v>
       </c>
     </row>
     <row r="22" spans="1:2" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A22" s="21">
-        <v>45397</v>
+        <v>45427</v>
       </c>
       <c r="B22" s="16">
-        <v>45397</v>
+        <v>45427</v>
       </c>
     </row>
     <row r="23" spans="1:2" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A23" s="21">
-        <v>45398</v>
+        <v>45428</v>
       </c>
       <c r="B23" s="16">
-        <v>45398</v>
+        <v>45428</v>
       </c>
     </row>
     <row r="24" spans="1:2" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A24" s="21">
-        <v>45399</v>
+        <v>45429</v>
       </c>
       <c r="B24" s="16">
-        <v>45399</v>
+        <v>45429</v>
       </c>
     </row>
     <row r="25" spans="1:2" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A25" s="21">
-        <v>45400</v>
+        <v>45432</v>
       </c>
       <c r="B25" s="16">
-        <v>45400</v>
+        <v>45432</v>
       </c>
     </row>
     <row r="26" spans="1:2" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A26" s="21">
-        <v>45401</v>
+        <v>45433</v>
       </c>
       <c r="B26" s="16">
-        <v>45401</v>
+        <v>45433</v>
       </c>
     </row>
     <row r="27" spans="1:2" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A27" s="21">
-        <v>45404</v>
+        <v>45434</v>
       </c>
       <c r="B27" s="16">
-        <v>45404</v>
+        <v>45434</v>
       </c>
     </row>
     <row r="28" spans="1:2" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A28" s="21">
-        <v>45405</v>
+        <v>45435</v>
       </c>
       <c r="B28" s="16">
-        <v>45405</v>
+        <v>45435</v>
       </c>
     </row>
     <row r="29" spans="1:2" ht="30" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A29" s="21" t="str">
-        <v/>
-      </c>
-      <c r="B29" s="16" t="str">
-        <v/>
+      <c r="A29" s="21">
+        <v>45436</v>
+      </c>
+      <c r="B29" s="16">
+        <v>45436</v>
       </c>
     </row>
     <row r="30" spans="1:2" ht="30" customHeight="1" x14ac:dyDescent="0.35">
@@ -1000,42 +1000,42 @@
     </row>
     <row r="31" spans="1:2" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A31" s="23">
-        <v>45406</v>
+        <v>45439</v>
       </c>
       <c r="B31" s="16">
-        <v>45406</v>
+        <v>45439</v>
       </c>
     </row>
     <row r="32" spans="1:2" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A32" s="23">
-        <v>45407</v>
+        <v>45440</v>
       </c>
       <c r="B32" s="16">
-        <v>45407</v>
+        <v>45440</v>
       </c>
     </row>
     <row r="33" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A33" s="23">
-        <v>45408</v>
+        <v>45441</v>
       </c>
       <c r="B33" s="16">
-        <v>45408</v>
+        <v>45441</v>
       </c>
     </row>
     <row r="34" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A34" s="21">
-        <v>45411</v>
+        <v>45442</v>
       </c>
       <c r="B34" s="22">
-        <v>45411</v>
+        <v>45442</v>
       </c>
     </row>
     <row r="35" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A35" s="23">
-        <v>45412</v>
+        <v>45443</v>
       </c>
       <c r="B35" s="16">
-        <v>45412</v>
+        <v>45443</v>
       </c>
     </row>
     <row r="36" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.35">
@@ -3926,7 +3926,7 @@
     <row r="1" spans="2:11" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B1" s="36">
         <f>DATEVALUE('999'!$F$8 &amp; " 1, " &amp; '999'!$H$8)</f>
-        <v>45383</v>
+        <v>45413</v>
       </c>
       <c r="C1" s="36"/>
       <c r="E1" s="37" t="s">
@@ -3951,26 +3951,26 @@
         <v>1</v>
       </c>
       <c r="E2" s="25" cm="1">
-        <f t="array" ref="E2:E31">IF(B8=FALSE, _xlfn.SEQUENCE(DAY(EOMONTH(B1,0)), 1,B1, 1), "")</f>
-        <v>45383</v>
+        <f t="array" ref="E2:E32">IF(B8=FALSE, _xlfn.SEQUENCE(DAY(EOMONTH(B1,0)), 1,B1, 1), "")</f>
+        <v>45413</v>
       </c>
       <c r="F2" s="27">
         <f>IF($E2="","",WEEKDAY($E2)-1)</f>
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="G2" s="6"/>
       <c r="H2" s="25" cm="1">
-        <f t="array" ref="H2:H23">_xlfn._xlws.FILTER($E$2:$E$32, ($F$2:$F$32=$C$2)+($F$2:$F$32=$C$3)+($F$2:$F$32=$C$4)+($F$2:$F$32=$C$5)+($F$2:$F$32=$C$6)+($F$2:$F$32=$C$7), "")</f>
-        <v>45383</v>
+        <f t="array" ref="H2:H24">_xlfn._xlws.FILTER($E$2:$E$32, ($F$2:$F$32=$C$2)+($F$2:$F$32=$C$3)+($F$2:$F$32=$C$4)+($F$2:$F$32=$C$5)+($F$2:$F$32=$C$6)+($F$2:$F$32=$C$7), "")</f>
+        <v>45413</v>
       </c>
       <c r="I2" s="6"/>
       <c r="J2" s="19" cm="1">
-        <f t="array" ref="J2:J18">IF(OR(ISBLANK($H$21), $H$26&lt;&gt;""), _xlfn._xlws.FILTER($H$2:$H$32, (ROW($H$2:$H$32)&lt;21)*($H$2:$H$32&lt;&gt;"")), _xlfn._xlws.FILTER($H$2:$H$32, (ROW($H$2:$H$32)&lt;=COUNT($H$2:$H$32)-4)*($H$2:$H$32&lt;&gt;"")))</f>
-        <v>45383</v>
+        <f t="array" ref="J2:J19">IF(OR(ISBLANK($H$21), $H$26&lt;&gt;""), _xlfn._xlws.FILTER($H$2:$H$32, (ROW($H$2:$H$32)&lt;21)*($H$2:$H$32&lt;&gt;"")), _xlfn._xlws.FILTER($H$2:$H$32, (ROW($H$2:$H$32)&lt;=COUNT($H$2:$H$32)-4)*($H$2:$H$32&lt;&gt;"")))</f>
+        <v>45413</v>
       </c>
       <c r="K2" s="13" cm="1">
-        <f t="array" ref="K2:K18">IF(OR(ISBLANK($H$21), $H$26&lt;&gt;""), _xlfn._xlws.FILTER($H$2:$H$32, (ROW($H$2:$H$32)&lt;21)*($H$2:$H$32&lt;&gt;"")), _xlfn._xlws.FILTER($H$2:$H$32, (ROW($H$2:$H$32)&lt;=COUNT($H$2:$H$32)-4)*($H$2:$H$32&lt;&gt;"")))</f>
-        <v>45383</v>
+        <f t="array" ref="K2:K19">IF(OR(ISBLANK($H$21), $H$26&lt;&gt;""), _xlfn._xlws.FILTER($H$2:$H$32, (ROW($H$2:$H$32)&lt;21)*($H$2:$H$32&lt;&gt;"")), _xlfn._xlws.FILTER($H$2:$H$32, (ROW($H$2:$H$32)&lt;=COUNT($H$2:$H$32)-4)*($H$2:$H$32&lt;&gt;"")))</f>
+        <v>45413</v>
       </c>
     </row>
     <row r="3" spans="2:11" ht="14.5" x14ac:dyDescent="0.35">
@@ -3982,22 +3982,22 @@
         <v>2</v>
       </c>
       <c r="E3" s="4">
-        <v>45384</v>
+        <v>45414</v>
       </c>
       <c r="F3" s="5">
         <f t="shared" ref="F3:F32" si="1">IF($E3="","",WEEKDAY($E3)-1)</f>
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="G3" s="6"/>
       <c r="H3" s="4">
-        <v>45384</v>
+        <v>45414</v>
       </c>
       <c r="I3" s="6"/>
       <c r="J3" s="19">
-        <v>45384</v>
+        <v>45414</v>
       </c>
       <c r="K3" s="13">
-        <v>45384</v>
+        <v>45414</v>
       </c>
     </row>
     <row r="4" spans="2:11" ht="14.5" x14ac:dyDescent="0.35">
@@ -4009,22 +4009,22 @@
         <v>3</v>
       </c>
       <c r="E4" s="4">
-        <v>45385</v>
+        <v>45415</v>
       </c>
       <c r="F4" s="5">
         <f t="shared" si="1"/>
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="G4" s="6"/>
       <c r="H4" s="4">
-        <v>45385</v>
+        <v>45415</v>
       </c>
       <c r="I4" s="6"/>
       <c r="J4" s="19">
-        <v>45385</v>
+        <v>45415</v>
       </c>
       <c r="K4" s="13">
-        <v>45385</v>
+        <v>45415</v>
       </c>
     </row>
     <row r="5" spans="2:11" ht="14.5" x14ac:dyDescent="0.35">
@@ -4036,22 +4036,22 @@
         <v>4</v>
       </c>
       <c r="E5" s="4">
-        <v>45386</v>
+        <v>45416</v>
       </c>
       <c r="F5" s="5">
         <f t="shared" si="1"/>
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="G5" s="6"/>
       <c r="H5" s="4">
-        <v>45386</v>
+        <v>45418</v>
       </c>
       <c r="I5" s="6"/>
       <c r="J5" s="19">
-        <v>45386</v>
+        <v>45418</v>
       </c>
       <c r="K5" s="13">
-        <v>45386</v>
+        <v>45418</v>
       </c>
     </row>
     <row r="6" spans="2:11" ht="14.5" x14ac:dyDescent="0.35">
@@ -4063,22 +4063,22 @@
         <v>5</v>
       </c>
       <c r="E6" s="4">
-        <v>45387</v>
+        <v>45417</v>
       </c>
       <c r="F6" s="5">
         <f t="shared" si="1"/>
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="G6" s="6"/>
       <c r="H6" s="4">
-        <v>45387</v>
+        <v>45419</v>
       </c>
       <c r="I6" s="6"/>
       <c r="J6" s="19">
-        <v>45387</v>
+        <v>45419</v>
       </c>
       <c r="K6" s="13">
-        <v>45387</v>
+        <v>45419</v>
       </c>
     </row>
     <row r="7" spans="2:11" ht="14.5" x14ac:dyDescent="0.35">
@@ -4088,22 +4088,22 @@
         <v>-1</v>
       </c>
       <c r="E7" s="4">
-        <v>45388</v>
+        <v>45418</v>
       </c>
       <c r="F7" s="5">
         <f t="shared" si="1"/>
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="G7" s="6"/>
       <c r="H7" s="4">
-        <v>45390</v>
+        <v>45420</v>
       </c>
       <c r="I7" s="6"/>
       <c r="J7" s="19">
-        <v>45390</v>
+        <v>45420</v>
       </c>
       <c r="K7" s="13">
-        <v>45390</v>
+        <v>45420</v>
       </c>
     </row>
     <row r="8" spans="2:11" ht="14.5" x14ac:dyDescent="0.35">
@@ -4113,253 +4113,257 @@
       </c>
       <c r="C8" s="39"/>
       <c r="E8" s="4">
-        <v>45389</v>
+        <v>45419</v>
       </c>
       <c r="F8" s="5">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="G8" s="6"/>
       <c r="H8" s="4">
-        <v>45391</v>
+        <v>45421</v>
       </c>
       <c r="I8" s="6"/>
       <c r="J8" s="19">
-        <v>45391</v>
+        <v>45421</v>
       </c>
       <c r="K8" s="13">
-        <v>45391</v>
+        <v>45421</v>
       </c>
     </row>
     <row r="9" spans="2:11" ht="14.5" x14ac:dyDescent="0.35">
       <c r="B9" s="39"/>
       <c r="C9" s="39"/>
       <c r="E9" s="4">
-        <v>45390</v>
+        <v>45420</v>
       </c>
       <c r="F9" s="5">
         <f t="shared" si="1"/>
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="G9" s="6"/>
       <c r="H9" s="4">
-        <v>45392</v>
+        <v>45422</v>
       </c>
       <c r="I9" s="6"/>
       <c r="J9" s="19">
-        <v>45392</v>
+        <v>45422</v>
       </c>
       <c r="K9" s="13">
-        <v>45392</v>
+        <v>45422</v>
       </c>
     </row>
     <row r="10" spans="2:11" ht="14.5" x14ac:dyDescent="0.35">
       <c r="E10" s="4">
-        <v>45391</v>
+        <v>45421</v>
       </c>
       <c r="F10" s="5">
         <f t="shared" si="1"/>
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="G10" s="6"/>
       <c r="H10" s="4">
-        <v>45393</v>
+        <v>45425</v>
       </c>
       <c r="I10" s="6"/>
       <c r="J10" s="19">
-        <v>45393</v>
+        <v>45425</v>
       </c>
       <c r="K10" s="13">
-        <v>45393</v>
+        <v>45425</v>
       </c>
     </row>
     <row r="11" spans="2:11" ht="14.5" x14ac:dyDescent="0.35">
       <c r="E11" s="4">
-        <v>45392</v>
+        <v>45422</v>
       </c>
       <c r="F11" s="5">
         <f t="shared" si="1"/>
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="G11" s="6"/>
       <c r="H11" s="4">
-        <v>45394</v>
+        <v>45426</v>
       </c>
       <c r="I11" s="6"/>
       <c r="J11" s="19">
-        <v>45394</v>
+        <v>45426</v>
       </c>
       <c r="K11" s="13">
-        <v>45394</v>
+        <v>45426</v>
       </c>
     </row>
     <row r="12" spans="2:11" ht="14.5" x14ac:dyDescent="0.35">
       <c r="E12" s="4">
-        <v>45393</v>
+        <v>45423</v>
       </c>
       <c r="F12" s="5">
         <f t="shared" si="1"/>
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="G12" s="6"/>
       <c r="H12" s="4">
-        <v>45397</v>
+        <v>45427</v>
       </c>
       <c r="I12" s="6"/>
       <c r="J12" s="19">
-        <v>45397</v>
+        <v>45427</v>
       </c>
       <c r="K12" s="13">
-        <v>45397</v>
+        <v>45427</v>
       </c>
     </row>
     <row r="13" spans="2:11" ht="14.5" x14ac:dyDescent="0.35">
       <c r="E13" s="4">
-        <v>45394</v>
+        <v>45424</v>
       </c>
       <c r="F13" s="5">
         <f t="shared" si="1"/>
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="G13" s="6"/>
       <c r="H13" s="4">
-        <v>45398</v>
+        <v>45428</v>
       </c>
       <c r="I13" s="6"/>
       <c r="J13" s="19">
-        <v>45398</v>
+        <v>45428</v>
       </c>
       <c r="K13" s="13">
-        <v>45398</v>
+        <v>45428</v>
       </c>
     </row>
     <row r="14" spans="2:11" ht="14.5" x14ac:dyDescent="0.35">
       <c r="E14" s="4">
-        <v>45395</v>
+        <v>45425</v>
       </c>
       <c r="F14" s="5">
         <f t="shared" si="1"/>
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="G14" s="6"/>
       <c r="H14" s="4">
-        <v>45399</v>
+        <v>45429</v>
       </c>
       <c r="I14" s="6"/>
       <c r="J14" s="19">
-        <v>45399</v>
+        <v>45429</v>
       </c>
       <c r="K14" s="13">
-        <v>45399</v>
+        <v>45429</v>
       </c>
     </row>
     <row r="15" spans="2:11" ht="14.5" x14ac:dyDescent="0.35">
       <c r="E15" s="4">
-        <v>45396</v>
+        <v>45426</v>
       </c>
       <c r="F15" s="5">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="G15" s="6"/>
       <c r="H15" s="4">
-        <v>45400</v>
+        <v>45432</v>
       </c>
       <c r="I15" s="6"/>
       <c r="J15" s="19">
-        <v>45400</v>
+        <v>45432</v>
       </c>
       <c r="K15" s="13">
-        <v>45400</v>
+        <v>45432</v>
       </c>
     </row>
     <row r="16" spans="2:11" ht="14.5" x14ac:dyDescent="0.35">
       <c r="E16" s="4">
-        <v>45397</v>
+        <v>45427</v>
       </c>
       <c r="F16" s="5">
         <f t="shared" si="1"/>
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="G16" s="6"/>
       <c r="H16" s="4">
-        <v>45401</v>
+        <v>45433</v>
       </c>
       <c r="I16" s="6"/>
       <c r="J16" s="19">
-        <v>45401</v>
+        <v>45433</v>
       </c>
       <c r="K16" s="13">
-        <v>45401</v>
+        <v>45433</v>
       </c>
     </row>
     <row r="17" spans="5:11" ht="14.5" x14ac:dyDescent="0.35">
       <c r="E17" s="4">
-        <v>45398</v>
+        <v>45428</v>
       </c>
       <c r="F17" s="5">
         <f t="shared" si="1"/>
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="G17" s="6"/>
       <c r="H17" s="4">
-        <v>45404</v>
+        <v>45434</v>
       </c>
       <c r="I17" s="6"/>
       <c r="J17" s="19">
-        <v>45404</v>
+        <v>45434</v>
       </c>
       <c r="K17" s="13">
-        <v>45404</v>
+        <v>45434</v>
       </c>
     </row>
     <row r="18" spans="5:11" ht="14.5" x14ac:dyDescent="0.35">
       <c r="E18" s="4">
-        <v>45399</v>
+        <v>45429</v>
       </c>
       <c r="F18" s="5">
         <f t="shared" si="1"/>
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="G18" s="6"/>
       <c r="H18" s="4">
-        <v>45405</v>
+        <v>45435</v>
       </c>
       <c r="I18" s="6"/>
       <c r="J18" s="19">
-        <v>45405</v>
+        <v>45435</v>
       </c>
       <c r="K18" s="13">
-        <v>45405</v>
+        <v>45435</v>
       </c>
     </row>
     <row r="19" spans="5:11" ht="14.5" x14ac:dyDescent="0.35">
       <c r="E19" s="4">
-        <v>45400</v>
+        <v>45430</v>
       </c>
       <c r="F19" s="5">
         <f t="shared" si="1"/>
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="G19" s="6"/>
       <c r="H19" s="4">
-        <v>45406</v>
+        <v>45436</v>
       </c>
       <c r="I19" s="6"/>
-      <c r="J19" s="19"/>
-      <c r="K19" s="13"/>
+      <c r="J19" s="19">
+        <v>45436</v>
+      </c>
+      <c r="K19" s="13">
+        <v>45436</v>
+      </c>
     </row>
     <row r="20" spans="5:11" ht="14.5" x14ac:dyDescent="0.35">
       <c r="E20" s="4">
-        <v>45401</v>
+        <v>45431</v>
       </c>
       <c r="F20" s="5">
         <f t="shared" si="1"/>
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="G20" s="6"/>
       <c r="H20" s="4">
-        <v>45407</v>
+        <v>45439</v>
       </c>
       <c r="I20" s="6"/>
       <c r="J20" s="19"/>
@@ -4367,109 +4371,111 @@
     </row>
     <row r="21" spans="5:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E21" s="4">
-        <v>45402</v>
+        <v>45432</v>
       </c>
       <c r="F21" s="5">
         <f t="shared" si="1"/>
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="G21" s="6"/>
       <c r="H21" s="4">
-        <v>45408</v>
+        <v>45440</v>
       </c>
       <c r="I21" s="6"/>
       <c r="J21" s="19" cm="1">
         <f t="array" ref="J21:J25">IF(ISBLANK($H$21),"",IF(ISBLANK($H$26), _xlfn._xlws.FILTER($H$2:$H$32, (ROW($H$2:$H$32)&gt;COUNT($H$2:$H$32)-4)*($H$2:$H$32&lt;&gt;"")),_xlfn._xlws.FILTER($H$2:$H$32, (ROW($H$2:$H$32)&gt;=21)*($H$2:$H$32&lt;&gt;""))))</f>
-        <v>45406</v>
+        <v>45439</v>
       </c>
       <c r="K21" s="13" cm="1">
         <f t="array" ref="K21:K25">IF(ISBLANK($H$21),"",IF(ISBLANK($H$26), _xlfn._xlws.FILTER($H$2:$H$32, (ROW($H$2:$H$32)&gt;COUNT($H$2:$H$32)-4)*($H$2:$H$32&lt;&gt;"")),_xlfn._xlws.FILTER($H$2:$H$32, (ROW($H$2:$H$32)&gt;=20)*($H$2:$H$32&lt;&gt;""))))</f>
-        <v>45406</v>
+        <v>45439</v>
       </c>
     </row>
     <row r="22" spans="5:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E22" s="4">
-        <v>45403</v>
+        <v>45433</v>
       </c>
       <c r="F22" s="5">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="G22" s="6"/>
       <c r="H22" s="4">
-        <v>45411</v>
+        <v>45441</v>
       </c>
       <c r="I22" s="6"/>
       <c r="J22" s="19">
-        <v>45407</v>
+        <v>45440</v>
       </c>
       <c r="K22" s="13">
-        <v>45407</v>
+        <v>45440</v>
       </c>
     </row>
     <row r="23" spans="5:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E23" s="4">
-        <v>45404</v>
+        <v>45434</v>
       </c>
       <c r="F23" s="5">
         <f t="shared" si="1"/>
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="G23" s="6"/>
       <c r="H23" s="4">
-        <v>45412</v>
+        <v>45442</v>
       </c>
       <c r="I23" s="6"/>
       <c r="J23" s="19">
-        <v>45408</v>
+        <v>45441</v>
       </c>
       <c r="K23" s="13">
-        <v>45408</v>
+        <v>45441</v>
       </c>
     </row>
     <row r="24" spans="5:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E24" s="4">
-        <v>45405</v>
+        <v>45435</v>
       </c>
       <c r="F24" s="5">
         <f t="shared" si="1"/>
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="G24" s="6"/>
-      <c r="H24" s="4"/>
+      <c r="H24" s="4">
+        <v>45443</v>
+      </c>
       <c r="I24" s="6"/>
       <c r="J24" s="19">
-        <v>45411</v>
+        <v>45442</v>
       </c>
       <c r="K24" s="13">
-        <v>45411</v>
+        <v>45442</v>
       </c>
     </row>
     <row r="25" spans="5:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E25" s="4">
-        <v>45406</v>
+        <v>45436</v>
       </c>
       <c r="F25" s="5">
         <f t="shared" si="1"/>
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="G25" s="6"/>
       <c r="H25" s="4"/>
       <c r="I25" s="6"/>
       <c r="J25" s="19">
-        <v>45412</v>
+        <v>45443</v>
       </c>
       <c r="K25" s="13">
-        <v>45412</v>
+        <v>45443</v>
       </c>
     </row>
     <row r="26" spans="5:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E26" s="4">
-        <v>45407</v>
+        <v>45437</v>
       </c>
       <c r="F26" s="5">
         <f t="shared" si="1"/>
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="G26" s="6"/>
       <c r="H26" s="4"/>
@@ -4479,11 +4485,11 @@
     </row>
     <row r="27" spans="5:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E27" s="4">
-        <v>45408</v>
+        <v>45438</v>
       </c>
       <c r="F27" s="5">
         <f t="shared" si="1"/>
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="G27" s="6"/>
       <c r="H27" s="4"/>
@@ -4493,11 +4499,11 @@
     </row>
     <row r="28" spans="5:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E28" s="4">
-        <v>45409</v>
+        <v>45439</v>
       </c>
       <c r="F28" s="5">
         <f t="shared" si="1"/>
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="G28" s="6"/>
       <c r="H28" s="4"/>
@@ -4507,11 +4513,11 @@
     </row>
     <row r="29" spans="5:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E29" s="4">
-        <v>45410</v>
+        <v>45440</v>
       </c>
       <c r="F29" s="5">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="G29" s="6"/>
       <c r="H29" s="4"/>
@@ -4521,11 +4527,11 @@
     </row>
     <row r="30" spans="5:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E30" s="4">
-        <v>45411</v>
+        <v>45441</v>
       </c>
       <c r="F30" s="5">
         <f t="shared" si="1"/>
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="G30" s="6"/>
       <c r="H30" s="4"/>
@@ -4535,11 +4541,11 @@
     </row>
     <row r="31" spans="5:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E31" s="4">
-        <v>45412</v>
+        <v>45442</v>
       </c>
       <c r="F31" s="5">
         <f t="shared" si="1"/>
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="G31" s="6"/>
       <c r="H31" s="4"/>
@@ -4548,10 +4554,12 @@
       <c r="K31" s="13"/>
     </row>
     <row r="32" spans="5:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="E32" s="4"/>
-      <c r="F32" s="5" t="str">
+      <c r="E32" s="4">
+        <v>45443</v>
+      </c>
+      <c r="F32" s="5">
         <f t="shared" si="1"/>
-        <v/>
+        <v>5</v>
       </c>
       <c r="G32" s="6"/>
       <c r="H32" s="4"/>

</xml_diff>

<commit_message>
Print 1st sheet only
</commit_message>
<xml_diff>
--- a/templateNew.xlsx
+++ b/templateNew.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27425"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27531"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Kai\Desktop\TimeSheet\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{4D73AB3B-8D0F-484D-BF62-8271640986ED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{BD056AA7-0C01-4866-9E95-6ACD93166912}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3040" yWindow="3040" windowWidth="19200" windowHeight="10060" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="380" yWindow="380" windowWidth="19200" windowHeight="10060" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="999" sheetId="3" r:id="rId1"/>
@@ -129,7 +129,7 @@
     <t>VERY GOOD BUILDING COMPANY</t>
   </si>
   <si>
-    <t>MAY</t>
+    <t>JUNE</t>
   </si>
 </sst>
 </file>
@@ -758,7 +758,7 @@
       <c r="G7" s="17"/>
       <c r="H7" s="17" t="str">
         <f>COUNTA(Formulas!H2:H30) &amp; " DAYS"</f>
-        <v>23 DAYS</v>
+        <v>20 DAYS</v>
       </c>
     </row>
     <row r="8" spans="1:8" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
@@ -842,10 +842,10 @@
     <row r="12" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A12" s="21" cm="1">
         <f t="array" ref="A12:B35">_xlfn._xlws.FILTER(IF(Formulas!$J$2:'Formulas'!$K$31&lt;&gt;0, Formulas!$J$2:'Formulas'!$K$31, ""), (ROW(Formulas!$J$2:'Formulas'!$J$31) &lt;= MAX(_xlfn._xlws.FILTER(ROW(Formulas!$J$2:'Formulas'!$J$31), Formulas!$J$2:'Formulas'!$J$31&lt;&gt;""))))</f>
-        <v>45413</v>
+        <v>45446</v>
       </c>
       <c r="B12" s="16">
-        <v>45413</v>
+        <v>45446</v>
       </c>
       <c r="C12" s="1"/>
       <c r="D12" s="1"/>
@@ -856,138 +856,138 @@
     </row>
     <row r="13" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A13" s="21">
-        <v>45414</v>
+        <v>45447</v>
       </c>
       <c r="B13" s="16">
-        <v>45414</v>
+        <v>45447</v>
       </c>
     </row>
     <row r="14" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A14" s="21">
-        <v>45415</v>
+        <v>45448</v>
       </c>
       <c r="B14" s="16">
-        <v>45415</v>
+        <v>45448</v>
       </c>
     </row>
     <row r="15" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A15" s="21">
-        <v>45418</v>
+        <v>45449</v>
       </c>
       <c r="B15" s="16">
-        <v>45418</v>
+        <v>45449</v>
       </c>
     </row>
     <row r="16" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A16" s="21">
-        <v>45419</v>
+        <v>45450</v>
       </c>
       <c r="B16" s="16">
-        <v>45419</v>
+        <v>45450</v>
       </c>
     </row>
     <row r="17" spans="1:2" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A17" s="21">
-        <v>45420</v>
+        <v>45453</v>
       </c>
       <c r="B17" s="16">
-        <v>45420</v>
+        <v>45453</v>
       </c>
     </row>
     <row r="18" spans="1:2" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A18" s="21">
-        <v>45421</v>
+        <v>45454</v>
       </c>
       <c r="B18" s="16">
-        <v>45421</v>
+        <v>45454</v>
       </c>
     </row>
     <row r="19" spans="1:2" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A19" s="21">
-        <v>45422</v>
+        <v>45455</v>
       </c>
       <c r="B19" s="16">
-        <v>45422</v>
+        <v>45455</v>
       </c>
     </row>
     <row r="20" spans="1:2" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A20" s="21">
-        <v>45425</v>
+        <v>45456</v>
       </c>
       <c r="B20" s="16">
-        <v>45425</v>
+        <v>45456</v>
       </c>
     </row>
     <row r="21" spans="1:2" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A21" s="21">
-        <v>45426</v>
+        <v>45457</v>
       </c>
       <c r="B21" s="16">
-        <v>45426</v>
+        <v>45457</v>
       </c>
     </row>
     <row r="22" spans="1:2" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A22" s="21">
-        <v>45427</v>
+        <v>45460</v>
       </c>
       <c r="B22" s="16">
-        <v>45427</v>
+        <v>45460</v>
       </c>
     </row>
     <row r="23" spans="1:2" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A23" s="21">
-        <v>45428</v>
+        <v>45461</v>
       </c>
       <c r="B23" s="16">
-        <v>45428</v>
+        <v>45461</v>
       </c>
     </row>
     <row r="24" spans="1:2" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A24" s="21">
-        <v>45429</v>
+        <v>45462</v>
       </c>
       <c r="B24" s="16">
-        <v>45429</v>
+        <v>45462</v>
       </c>
     </row>
     <row r="25" spans="1:2" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A25" s="21">
-        <v>45432</v>
+        <v>45463</v>
       </c>
       <c r="B25" s="16">
-        <v>45432</v>
+        <v>45463</v>
       </c>
     </row>
     <row r="26" spans="1:2" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A26" s="21">
-        <v>45433</v>
+        <v>45464</v>
       </c>
       <c r="B26" s="16">
-        <v>45433</v>
+        <v>45464</v>
       </c>
     </row>
     <row r="27" spans="1:2" ht="30" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A27" s="21">
-        <v>45434</v>
-      </c>
-      <c r="B27" s="16">
-        <v>45434</v>
+      <c r="A27" s="21" t="str">
+        <v/>
+      </c>
+      <c r="B27" s="16" t="str">
+        <v/>
       </c>
     </row>
     <row r="28" spans="1:2" ht="30" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A28" s="21">
-        <v>45435</v>
-      </c>
-      <c r="B28" s="16">
-        <v>45435</v>
+      <c r="A28" s="21" t="str">
+        <v/>
+      </c>
+      <c r="B28" s="16" t="str">
+        <v/>
       </c>
     </row>
     <row r="29" spans="1:2" ht="30" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A29" s="21">
-        <v>45436</v>
-      </c>
-      <c r="B29" s="16">
-        <v>45436</v>
+      <c r="A29" s="21" t="str">
+        <v/>
+      </c>
+      <c r="B29" s="16" t="str">
+        <v/>
       </c>
     </row>
     <row r="30" spans="1:2" ht="30" customHeight="1" x14ac:dyDescent="0.35">
@@ -1000,42 +1000,42 @@
     </row>
     <row r="31" spans="1:2" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A31" s="23">
-        <v>45439</v>
+        <v>45467</v>
       </c>
       <c r="B31" s="16">
-        <v>45439</v>
+        <v>45467</v>
       </c>
     </row>
     <row r="32" spans="1:2" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A32" s="23">
-        <v>45440</v>
+        <v>45468</v>
       </c>
       <c r="B32" s="16">
-        <v>45440</v>
+        <v>45468</v>
       </c>
     </row>
     <row r="33" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A33" s="23">
-        <v>45441</v>
+        <v>45469</v>
       </c>
       <c r="B33" s="16">
-        <v>45441</v>
+        <v>45469</v>
       </c>
     </row>
     <row r="34" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A34" s="21">
-        <v>45442</v>
+        <v>45470</v>
       </c>
       <c r="B34" s="22">
-        <v>45442</v>
+        <v>45470</v>
       </c>
     </row>
     <row r="35" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A35" s="23">
-        <v>45443</v>
+        <v>45471</v>
       </c>
       <c r="B35" s="16">
-        <v>45443</v>
+        <v>45471</v>
       </c>
     </row>
     <row r="36" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.35">
@@ -3926,7 +3926,7 @@
     <row r="1" spans="2:11" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B1" s="36">
         <f>DATEVALUE('999'!$F$8 &amp; " 1, " &amp; '999'!$H$8)</f>
-        <v>45413</v>
+        <v>45444</v>
       </c>
       <c r="C1" s="36"/>
       <c r="E1" s="37" t="s">
@@ -3951,26 +3951,26 @@
         <v>1</v>
       </c>
       <c r="E2" s="25" cm="1">
-        <f t="array" ref="E2:E32">IF(B8=FALSE, _xlfn.SEQUENCE(DAY(EOMONTH(B1,0)), 1,B1, 1), "")</f>
-        <v>45413</v>
+        <f t="array" ref="E2:E31">IF(B8=FALSE, _xlfn.SEQUENCE(DAY(EOMONTH(B1,0)), 1,B1, 1), "")</f>
+        <v>45444</v>
       </c>
       <c r="F2" s="27">
         <f>IF($E2="","",WEEKDAY($E2)-1)</f>
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="G2" s="6"/>
       <c r="H2" s="25" cm="1">
-        <f t="array" ref="H2:H24">_xlfn._xlws.FILTER($E$2:$E$32, ($F$2:$F$32=$C$2)+($F$2:$F$32=$C$3)+($F$2:$F$32=$C$4)+($F$2:$F$32=$C$5)+($F$2:$F$32=$C$6)+($F$2:$F$32=$C$7), "")</f>
-        <v>45413</v>
+        <f t="array" ref="H2:H21">_xlfn._xlws.FILTER($E$2:$E$32, ($F$2:$F$32=$C$2)+($F$2:$F$32=$C$3)+($F$2:$F$32=$C$4)+($F$2:$F$32=$C$5)+($F$2:$F$32=$C$6)+($F$2:$F$32=$C$7), "")</f>
+        <v>45446</v>
       </c>
       <c r="I2" s="6"/>
       <c r="J2" s="19" cm="1">
-        <f t="array" ref="J2:J19">IF(OR(ISBLANK($H$21), $H$26&lt;&gt;""), _xlfn._xlws.FILTER($H$2:$H$32, (ROW($H$2:$H$32)&lt;21)*($H$2:$H$32&lt;&gt;"")), _xlfn._xlws.FILTER($H$2:$H$32, (ROW($H$2:$H$32)&lt;=COUNT($H$2:$H$32)-4)*($H$2:$H$32&lt;&gt;"")))</f>
-        <v>45413</v>
+        <f t="array" ref="J2:J16">IF(OR(ISBLANK($H$21), $H$26&lt;&gt;""), _xlfn._xlws.FILTER($H$2:$H$32, (ROW($H$2:$H$32)&lt;21)*($H$2:$H$32&lt;&gt;"")), _xlfn._xlws.FILTER($H$2:$H$32, (ROW($H$2:$H$32)&lt;=COUNT($H$2:$H$32)-4)*($H$2:$H$32&lt;&gt;"")))</f>
+        <v>45446</v>
       </c>
       <c r="K2" s="13" cm="1">
-        <f t="array" ref="K2:K19">IF(OR(ISBLANK($H$21), $H$26&lt;&gt;""), _xlfn._xlws.FILTER($H$2:$H$32, (ROW($H$2:$H$32)&lt;21)*($H$2:$H$32&lt;&gt;"")), _xlfn._xlws.FILTER($H$2:$H$32, (ROW($H$2:$H$32)&lt;=COUNT($H$2:$H$32)-4)*($H$2:$H$32&lt;&gt;"")))</f>
-        <v>45413</v>
+        <f t="array" ref="K2:K16">IF(OR(ISBLANK($H$21), $H$26&lt;&gt;""), _xlfn._xlws.FILTER($H$2:$H$32, (ROW($H$2:$H$32)&lt;21)*($H$2:$H$32&lt;&gt;"")), _xlfn._xlws.FILTER($H$2:$H$32, (ROW($H$2:$H$32)&lt;=COUNT($H$2:$H$32)-4)*($H$2:$H$32&lt;&gt;"")))</f>
+        <v>45446</v>
       </c>
     </row>
     <row r="3" spans="2:11" ht="14.5" x14ac:dyDescent="0.35">
@@ -3982,22 +3982,22 @@
         <v>2</v>
       </c>
       <c r="E3" s="4">
-        <v>45414</v>
+        <v>45445</v>
       </c>
       <c r="F3" s="5">
         <f t="shared" ref="F3:F32" si="1">IF($E3="","",WEEKDAY($E3)-1)</f>
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="G3" s="6"/>
       <c r="H3" s="4">
-        <v>45414</v>
+        <v>45447</v>
       </c>
       <c r="I3" s="6"/>
       <c r="J3" s="19">
-        <v>45414</v>
+        <v>45447</v>
       </c>
       <c r="K3" s="13">
-        <v>45414</v>
+        <v>45447</v>
       </c>
     </row>
     <row r="4" spans="2:11" ht="14.5" x14ac:dyDescent="0.35">
@@ -4009,22 +4009,22 @@
         <v>3</v>
       </c>
       <c r="E4" s="4">
-        <v>45415</v>
+        <v>45446</v>
       </c>
       <c r="F4" s="5">
         <f t="shared" si="1"/>
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="G4" s="6"/>
       <c r="H4" s="4">
-        <v>45415</v>
+        <v>45448</v>
       </c>
       <c r="I4" s="6"/>
       <c r="J4" s="19">
-        <v>45415</v>
+        <v>45448</v>
       </c>
       <c r="K4" s="13">
-        <v>45415</v>
+        <v>45448</v>
       </c>
     </row>
     <row r="5" spans="2:11" ht="14.5" x14ac:dyDescent="0.35">
@@ -4036,22 +4036,22 @@
         <v>4</v>
       </c>
       <c r="E5" s="4">
-        <v>45416</v>
+        <v>45447</v>
       </c>
       <c r="F5" s="5">
         <f t="shared" si="1"/>
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="G5" s="6"/>
       <c r="H5" s="4">
-        <v>45418</v>
+        <v>45449</v>
       </c>
       <c r="I5" s="6"/>
       <c r="J5" s="19">
-        <v>45418</v>
+        <v>45449</v>
       </c>
       <c r="K5" s="13">
-        <v>45418</v>
+        <v>45449</v>
       </c>
     </row>
     <row r="6" spans="2:11" ht="14.5" x14ac:dyDescent="0.35">
@@ -4063,22 +4063,22 @@
         <v>5</v>
       </c>
       <c r="E6" s="4">
-        <v>45417</v>
+        <v>45448</v>
       </c>
       <c r="F6" s="5">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="G6" s="6"/>
       <c r="H6" s="4">
-        <v>45419</v>
+        <v>45450</v>
       </c>
       <c r="I6" s="6"/>
       <c r="J6" s="19">
-        <v>45419</v>
+        <v>45450</v>
       </c>
       <c r="K6" s="13">
-        <v>45419</v>
+        <v>45450</v>
       </c>
     </row>
     <row r="7" spans="2:11" ht="14.5" x14ac:dyDescent="0.35">
@@ -4088,22 +4088,22 @@
         <v>-1</v>
       </c>
       <c r="E7" s="4">
-        <v>45418</v>
+        <v>45449</v>
       </c>
       <c r="F7" s="5">
         <f t="shared" si="1"/>
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="G7" s="6"/>
       <c r="H7" s="4">
-        <v>45420</v>
+        <v>45453</v>
       </c>
       <c r="I7" s="6"/>
       <c r="J7" s="19">
-        <v>45420</v>
+        <v>45453</v>
       </c>
       <c r="K7" s="13">
-        <v>45420</v>
+        <v>45453</v>
       </c>
     </row>
     <row r="8" spans="2:11" ht="14.5" x14ac:dyDescent="0.35">
@@ -4113,257 +4113,245 @@
       </c>
       <c r="C8" s="39"/>
       <c r="E8" s="4">
-        <v>45419</v>
+        <v>45450</v>
       </c>
       <c r="F8" s="5">
         <f t="shared" si="1"/>
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="G8" s="6"/>
       <c r="H8" s="4">
-        <v>45421</v>
+        <v>45454</v>
       </c>
       <c r="I8" s="6"/>
       <c r="J8" s="19">
-        <v>45421</v>
+        <v>45454</v>
       </c>
       <c r="K8" s="13">
-        <v>45421</v>
+        <v>45454</v>
       </c>
     </row>
     <row r="9" spans="2:11" ht="14.5" x14ac:dyDescent="0.35">
       <c r="B9" s="39"/>
       <c r="C9" s="39"/>
       <c r="E9" s="4">
-        <v>45420</v>
+        <v>45451</v>
       </c>
       <c r="F9" s="5">
         <f t="shared" si="1"/>
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="G9" s="6"/>
       <c r="H9" s="4">
-        <v>45422</v>
+        <v>45455</v>
       </c>
       <c r="I9" s="6"/>
       <c r="J9" s="19">
-        <v>45422</v>
+        <v>45455</v>
       </c>
       <c r="K9" s="13">
-        <v>45422</v>
+        <v>45455</v>
       </c>
     </row>
     <row r="10" spans="2:11" ht="14.5" x14ac:dyDescent="0.35">
       <c r="E10" s="4">
-        <v>45421</v>
+        <v>45452</v>
       </c>
       <c r="F10" s="5">
         <f t="shared" si="1"/>
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="G10" s="6"/>
       <c r="H10" s="4">
-        <v>45425</v>
+        <v>45456</v>
       </c>
       <c r="I10" s="6"/>
       <c r="J10" s="19">
-        <v>45425</v>
+        <v>45456</v>
       </c>
       <c r="K10" s="13">
-        <v>45425</v>
+        <v>45456</v>
       </c>
     </row>
     <row r="11" spans="2:11" ht="14.5" x14ac:dyDescent="0.35">
       <c r="E11" s="4">
-        <v>45422</v>
+        <v>45453</v>
       </c>
       <c r="F11" s="5">
         <f t="shared" si="1"/>
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="G11" s="6"/>
       <c r="H11" s="4">
-        <v>45426</v>
+        <v>45457</v>
       </c>
       <c r="I11" s="6"/>
       <c r="J11" s="19">
-        <v>45426</v>
+        <v>45457</v>
       </c>
       <c r="K11" s="13">
-        <v>45426</v>
+        <v>45457</v>
       </c>
     </row>
     <row r="12" spans="2:11" ht="14.5" x14ac:dyDescent="0.35">
       <c r="E12" s="4">
-        <v>45423</v>
+        <v>45454</v>
       </c>
       <c r="F12" s="5">
         <f t="shared" si="1"/>
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="G12" s="6"/>
       <c r="H12" s="4">
-        <v>45427</v>
+        <v>45460</v>
       </c>
       <c r="I12" s="6"/>
       <c r="J12" s="19">
-        <v>45427</v>
+        <v>45460</v>
       </c>
       <c r="K12" s="13">
-        <v>45427</v>
+        <v>45460</v>
       </c>
     </row>
     <row r="13" spans="2:11" ht="14.5" x14ac:dyDescent="0.35">
       <c r="E13" s="4">
-        <v>45424</v>
+        <v>45455</v>
       </c>
       <c r="F13" s="5">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="G13" s="6"/>
       <c r="H13" s="4">
-        <v>45428</v>
+        <v>45461</v>
       </c>
       <c r="I13" s="6"/>
       <c r="J13" s="19">
-        <v>45428</v>
+        <v>45461</v>
       </c>
       <c r="K13" s="13">
-        <v>45428</v>
+        <v>45461</v>
       </c>
     </row>
     <row r="14" spans="2:11" ht="14.5" x14ac:dyDescent="0.35">
       <c r="E14" s="4">
-        <v>45425</v>
+        <v>45456</v>
       </c>
       <c r="F14" s="5">
         <f t="shared" si="1"/>
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="G14" s="6"/>
       <c r="H14" s="4">
-        <v>45429</v>
+        <v>45462</v>
       </c>
       <c r="I14" s="6"/>
       <c r="J14" s="19">
-        <v>45429</v>
+        <v>45462</v>
       </c>
       <c r="K14" s="13">
-        <v>45429</v>
+        <v>45462</v>
       </c>
     </row>
     <row r="15" spans="2:11" ht="14.5" x14ac:dyDescent="0.35">
       <c r="E15" s="4">
-        <v>45426</v>
+        <v>45457</v>
       </c>
       <c r="F15" s="5">
         <f t="shared" si="1"/>
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="G15" s="6"/>
       <c r="H15" s="4">
-        <v>45432</v>
+        <v>45463</v>
       </c>
       <c r="I15" s="6"/>
       <c r="J15" s="19">
-        <v>45432</v>
+        <v>45463</v>
       </c>
       <c r="K15" s="13">
-        <v>45432</v>
+        <v>45463</v>
       </c>
     </row>
     <row r="16" spans="2:11" ht="14.5" x14ac:dyDescent="0.35">
       <c r="E16" s="4">
-        <v>45427</v>
+        <v>45458</v>
       </c>
       <c r="F16" s="5">
         <f t="shared" si="1"/>
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="G16" s="6"/>
       <c r="H16" s="4">
-        <v>45433</v>
+        <v>45464</v>
       </c>
       <c r="I16" s="6"/>
       <c r="J16" s="19">
-        <v>45433</v>
+        <v>45464</v>
       </c>
       <c r="K16" s="13">
-        <v>45433</v>
+        <v>45464</v>
       </c>
     </row>
     <row r="17" spans="5:11" ht="14.5" x14ac:dyDescent="0.35">
       <c r="E17" s="4">
-        <v>45428</v>
+        <v>45459</v>
       </c>
       <c r="F17" s="5">
         <f t="shared" si="1"/>
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="G17" s="6"/>
       <c r="H17" s="4">
-        <v>45434</v>
+        <v>45467</v>
       </c>
       <c r="I17" s="6"/>
-      <c r="J17" s="19">
-        <v>45434</v>
-      </c>
-      <c r="K17" s="13">
-        <v>45434</v>
-      </c>
+      <c r="J17" s="19"/>
+      <c r="K17" s="13"/>
     </row>
     <row r="18" spans="5:11" ht="14.5" x14ac:dyDescent="0.35">
       <c r="E18" s="4">
-        <v>45429</v>
+        <v>45460</v>
       </c>
       <c r="F18" s="5">
         <f t="shared" si="1"/>
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="G18" s="6"/>
       <c r="H18" s="4">
-        <v>45435</v>
+        <v>45468</v>
       </c>
       <c r="I18" s="6"/>
-      <c r="J18" s="19">
-        <v>45435</v>
-      </c>
-      <c r="K18" s="13">
-        <v>45435</v>
-      </c>
+      <c r="J18" s="19"/>
+      <c r="K18" s="13"/>
     </row>
     <row r="19" spans="5:11" ht="14.5" x14ac:dyDescent="0.35">
       <c r="E19" s="4">
-        <v>45430</v>
+        <v>45461</v>
       </c>
       <c r="F19" s="5">
         <f t="shared" si="1"/>
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="G19" s="6"/>
       <c r="H19" s="4">
-        <v>45436</v>
+        <v>45469</v>
       </c>
       <c r="I19" s="6"/>
-      <c r="J19" s="19">
-        <v>45436</v>
-      </c>
-      <c r="K19" s="13">
-        <v>45436</v>
-      </c>
+      <c r="J19" s="19"/>
+      <c r="K19" s="13"/>
     </row>
     <row r="20" spans="5:11" ht="14.5" x14ac:dyDescent="0.35">
       <c r="E20" s="4">
-        <v>45431</v>
+        <v>45462</v>
       </c>
       <c r="F20" s="5">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="G20" s="6"/>
       <c r="H20" s="4">
-        <v>45439</v>
+        <v>45470</v>
       </c>
       <c r="I20" s="6"/>
       <c r="J20" s="19"/>
@@ -4371,111 +4359,105 @@
     </row>
     <row r="21" spans="5:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E21" s="4">
-        <v>45432</v>
+        <v>45463</v>
       </c>
       <c r="F21" s="5">
         <f t="shared" si="1"/>
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="G21" s="6"/>
       <c r="H21" s="4">
-        <v>45440</v>
+        <v>45471</v>
       </c>
       <c r="I21" s="6"/>
       <c r="J21" s="19" cm="1">
         <f t="array" ref="J21:J25">IF(ISBLANK($H$21),"",IF(ISBLANK($H$26), _xlfn._xlws.FILTER($H$2:$H$32, (ROW($H$2:$H$32)&gt;COUNT($H$2:$H$32)-4)*($H$2:$H$32&lt;&gt;"")),_xlfn._xlws.FILTER($H$2:$H$32, (ROW($H$2:$H$32)&gt;=21)*($H$2:$H$32&lt;&gt;""))))</f>
-        <v>45439</v>
+        <v>45467</v>
       </c>
       <c r="K21" s="13" cm="1">
         <f t="array" ref="K21:K25">IF(ISBLANK($H$21),"",IF(ISBLANK($H$26), _xlfn._xlws.FILTER($H$2:$H$32, (ROW($H$2:$H$32)&gt;COUNT($H$2:$H$32)-4)*($H$2:$H$32&lt;&gt;"")),_xlfn._xlws.FILTER($H$2:$H$32, (ROW($H$2:$H$32)&gt;=20)*($H$2:$H$32&lt;&gt;""))))</f>
-        <v>45439</v>
+        <v>45467</v>
       </c>
     </row>
     <row r="22" spans="5:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E22" s="4">
-        <v>45433</v>
+        <v>45464</v>
       </c>
       <c r="F22" s="5">
         <f t="shared" si="1"/>
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="G22" s="6"/>
-      <c r="H22" s="4">
-        <v>45441</v>
-      </c>
+      <c r="H22" s="4"/>
       <c r="I22" s="6"/>
       <c r="J22" s="19">
-        <v>45440</v>
+        <v>45468</v>
       </c>
       <c r="K22" s="13">
-        <v>45440</v>
+        <v>45468</v>
       </c>
     </row>
     <row r="23" spans="5:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E23" s="4">
-        <v>45434</v>
+        <v>45465</v>
       </c>
       <c r="F23" s="5">
         <f t="shared" si="1"/>
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="G23" s="6"/>
-      <c r="H23" s="4">
-        <v>45442</v>
-      </c>
+      <c r="H23" s="4"/>
       <c r="I23" s="6"/>
       <c r="J23" s="19">
-        <v>45441</v>
+        <v>45469</v>
       </c>
       <c r="K23" s="13">
-        <v>45441</v>
+        <v>45469</v>
       </c>
     </row>
     <row r="24" spans="5:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E24" s="4">
-        <v>45435</v>
+        <v>45466</v>
       </c>
       <c r="F24" s="5">
         <f t="shared" si="1"/>
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="G24" s="6"/>
-      <c r="H24" s="4">
-        <v>45443</v>
-      </c>
+      <c r="H24" s="4"/>
       <c r="I24" s="6"/>
       <c r="J24" s="19">
-        <v>45442</v>
+        <v>45470</v>
       </c>
       <c r="K24" s="13">
-        <v>45442</v>
+        <v>45470</v>
       </c>
     </row>
     <row r="25" spans="5:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E25" s="4">
-        <v>45436</v>
+        <v>45467</v>
       </c>
       <c r="F25" s="5">
         <f t="shared" si="1"/>
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="G25" s="6"/>
       <c r="H25" s="4"/>
       <c r="I25" s="6"/>
       <c r="J25" s="19">
-        <v>45443</v>
+        <v>45471</v>
       </c>
       <c r="K25" s="13">
-        <v>45443</v>
+        <v>45471</v>
       </c>
     </row>
     <row r="26" spans="5:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E26" s="4">
-        <v>45437</v>
+        <v>45468</v>
       </c>
       <c r="F26" s="5">
         <f t="shared" si="1"/>
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="G26" s="6"/>
       <c r="H26" s="4"/>
@@ -4485,11 +4467,11 @@
     </row>
     <row r="27" spans="5:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E27" s="4">
-        <v>45438</v>
+        <v>45469</v>
       </c>
       <c r="F27" s="5">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="G27" s="6"/>
       <c r="H27" s="4"/>
@@ -4499,11 +4481,11 @@
     </row>
     <row r="28" spans="5:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E28" s="4">
-        <v>45439</v>
+        <v>45470</v>
       </c>
       <c r="F28" s="5">
         <f t="shared" si="1"/>
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="G28" s="6"/>
       <c r="H28" s="4"/>
@@ -4513,11 +4495,11 @@
     </row>
     <row r="29" spans="5:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E29" s="4">
-        <v>45440</v>
+        <v>45471</v>
       </c>
       <c r="F29" s="5">
         <f t="shared" si="1"/>
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="G29" s="6"/>
       <c r="H29" s="4"/>
@@ -4527,11 +4509,11 @@
     </row>
     <row r="30" spans="5:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E30" s="4">
-        <v>45441</v>
+        <v>45472</v>
       </c>
       <c r="F30" s="5">
         <f t="shared" si="1"/>
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="G30" s="6"/>
       <c r="H30" s="4"/>
@@ -4541,11 +4523,11 @@
     </row>
     <row r="31" spans="5:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E31" s="4">
-        <v>45442</v>
+        <v>45473</v>
       </c>
       <c r="F31" s="5">
         <f t="shared" si="1"/>
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="G31" s="6"/>
       <c r="H31" s="4"/>
@@ -4554,12 +4536,10 @@
       <c r="K31" s="13"/>
     </row>
     <row r="32" spans="5:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="E32" s="4">
-        <v>45443</v>
-      </c>
-      <c r="F32" s="5">
+      <c r="E32" s="4"/>
+      <c r="F32" s="5" t="str">
         <f t="shared" si="1"/>
-        <v>5</v>
+        <v/>
       </c>
       <c r="G32" s="6"/>
       <c r="H32" s="4"/>

</xml_diff>